<commit_message>
speaker added to the BOM
</commit_message>
<xml_diff>
--- a/Circuit design/Project Outputs for Circuit design/BOM.xlsx
+++ b/Circuit design/Project Outputs for Circuit design/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nilesh\UOM Projects\Hertz-Noise_Cancelling_Headphones\Circuit design\Project Outputs for Circuit design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BEC2804-53E2-4715-A9F4-5FA4188157BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1075A7FA-B5B7-4AFA-AE00-54A646072792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{0EB45293-B8D8-499C-BE47-6B5096D9A094}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="120">
   <si>
     <t>Line #</t>
   </si>
@@ -387,6 +387,18 @@
   </si>
   <si>
     <t>C20182914</t>
+  </si>
+  <si>
+    <t>Speaker</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>C49246995</t>
   </si>
 </sst>
 </file>
@@ -783,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F7B51B-04D7-4A29-865F-8F9EC3387040}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1433,6 +1445,31 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>